<commit_message>
update info and added new house DAUYS
</commit_message>
<xml_diff>
--- a/GAKKU.xlsx
+++ b/GAKKU.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="79">
   <si>
     <t>APT_NUMBER</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>173.6</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>173.7</t>
   </si>
 </sst>
 </file>
@@ -268,12 +274,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -288,10 +300,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -594,17 +607,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L31"/>
+  <dimension ref="A3:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -630,7 +647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -655,7 +672,7 @@
       <c r="I4">
         <v>36563800</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>45648</v>
       </c>
       <c r="K4">
@@ -665,7 +682,7 @@
         <v>36563800</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -690,7 +707,7 @@
       <c r="I5">
         <v>37455600</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>45648</v>
       </c>
       <c r="K5">
@@ -700,7 +717,7 @@
         <v>37455600</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -725,7 +742,7 @@
       <c r="I6">
         <v>38439100</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <v>45648</v>
       </c>
       <c r="K6">
@@ -735,7 +752,7 @@
         <v>38439100</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -760,7 +777,7 @@
       <c r="I7">
         <v>42483000</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <v>45648</v>
       </c>
       <c r="K7">
@@ -770,7 +787,7 @@
         <v>42483000</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -796,7 +813,7 @@
         <v>43726500</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -822,7 +839,7 @@
         <v>43911000</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -847,7 +864,7 @@
       <c r="I10">
         <v>56120000</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="1">
         <v>45648</v>
       </c>
       <c r="K10">
@@ -857,7 +874,7 @@
         <v>56120000</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -882,8 +899,26 @@
       <c r="I11">
         <v>72384000</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J11" s="2">
+        <v>45675</v>
+      </c>
+      <c r="K11" s="3">
+        <v>540000</v>
+      </c>
+      <c r="L11">
+        <v>75168000</v>
+      </c>
+      <c r="M11" s="2">
+        <v>45675</v>
+      </c>
+      <c r="N11">
+        <v>540000</v>
+      </c>
+      <c r="O11">
+        <v>75168000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -908,7 +943,7 @@
       <c r="I12">
         <v>75523500</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <v>45648</v>
       </c>
       <c r="K12">
@@ -917,8 +952,18 @@
       <c r="L12">
         <v>75523500</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="2">
+        <v>45675</v>
+      </c>
+      <c r="N12">
+        <v>585000</v>
+      </c>
+      <c r="O12">
+        <v>75523500</v>
+      </c>
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -943,7 +988,7 @@
       <c r="I13">
         <v>76590000</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
         <v>45648</v>
       </c>
       <c r="K13">
@@ -952,8 +997,18 @@
       <c r="L13">
         <v>76590000</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="2">
+        <v>45675</v>
+      </c>
+      <c r="N13">
+        <v>575000</v>
+      </c>
+      <c r="O13">
+        <v>76590000</v>
+      </c>
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -978,7 +1033,7 @@
       <c r="I14">
         <v>80163200</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="1">
         <v>45648</v>
       </c>
       <c r="K14">
@@ -988,7 +1043,7 @@
         <v>80163200</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1013,7 +1068,7 @@
       <c r="I15">
         <v>80166000</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="1">
         <v>45648</v>
       </c>
       <c r="K15">
@@ -1023,7 +1078,7 @@
         <v>80166000</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1049,7 +1104,7 @@
         <v>80224300</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1074,7 +1129,7 @@
       <c r="I17">
         <v>80353700</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="1">
         <v>45648</v>
       </c>
       <c r="K17">
@@ -1084,7 +1139,7 @@
         <v>80353700</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1109,7 +1164,7 @@
       <c r="I18">
         <v>80468700</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="1">
         <v>45648</v>
       </c>
       <c r="K18">
@@ -1119,7 +1174,7 @@
         <v>80468700</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -1145,7 +1200,7 @@
         <v>85858100</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -1170,7 +1225,7 @@
       <c r="I20">
         <v>87066000</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="1">
         <v>45648</v>
       </c>
       <c r="K20">
@@ -1179,8 +1234,18 @@
       <c r="L20">
         <v>87066000</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="2">
+        <v>45675</v>
+      </c>
+      <c r="N20">
+        <v>630000</v>
+      </c>
+      <c r="O20">
+        <v>87066000</v>
+      </c>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -1205,7 +1270,7 @@
       <c r="I21">
         <v>88072600</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="1">
         <v>45648</v>
       </c>
       <c r="K21">
@@ -1215,7 +1280,7 @@
         <v>88072600</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1240,7 +1305,7 @@
       <c r="I22">
         <v>88940500</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="1">
         <v>45648</v>
       </c>
       <c r="K22">
@@ -1250,7 +1315,7 @@
         <v>88940500</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -1276,7 +1341,7 @@
         <v>89095000</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -1302,7 +1367,7 @@
         <v>89146500</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -1327,7 +1392,7 @@
       <c r="I25">
         <v>89964000</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="1">
         <v>45648</v>
       </c>
       <c r="K25">
@@ -1337,7 +1402,7 @@
         <v>89964000</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -1362,7 +1427,7 @@
       <c r="I26">
         <v>90537000</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26" s="1">
         <v>45648</v>
       </c>
       <c r="K26">
@@ -1372,7 +1437,7 @@
         <v>90537000</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -1397,7 +1462,7 @@
       <c r="I27">
         <v>91263600</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J27" s="1">
         <v>45648</v>
       </c>
       <c r="K27">
@@ -1407,7 +1472,7 @@
         <v>91263600</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -1433,7 +1498,7 @@
         <v>91364000</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -1458,7 +1523,7 @@
       <c r="I29">
         <v>92355200</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29" s="1">
         <v>45648</v>
       </c>
       <c r="K29">
@@ -1468,7 +1533,7 @@
         <v>92355200</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -1493,7 +1558,7 @@
       <c r="I30">
         <v>93070800</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J30" s="1">
         <v>45648</v>
       </c>
       <c r="K30">
@@ -1503,7 +1568,7 @@
         <v>93070800</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -1527,6 +1592,41 @@
       </c>
       <c r="I31">
         <v>109368000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="2">
+        <v>45675</v>
+      </c>
+      <c r="H32">
+        <v>680000</v>
+      </c>
+      <c r="I32">
+        <v>118116000</v>
+      </c>
+      <c r="J32" s="2">
+        <v>45675</v>
+      </c>
+      <c r="K32">
+        <v>680000</v>
+      </c>
+      <c r="L32">
+        <v>118116000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>